<commit_message>
refactor chatbot search functionality to use API call and handle errors
</commit_message>
<xml_diff>
--- a/backend/data/faqs.xlsx
+++ b/backend/data/faqs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -19,29 +19,47 @@
     <t>Answer</t>
   </si>
   <si>
-    <t>What are your operating hours?</t>
-  </si>
-  <si>
-    <t>Bukas palagi never binabagyo</t>
-  </si>
-  <si>
-    <t>How can I book a cabin?</t>
-  </si>
-  <si>
-    <t>You can book a cabin through our website.</t>
-  </si>
-  <si>
-    <t>What is your cancellation policy?</t>
-  </si>
-  <si>
-    <t>Cancellations must be made 3 days in advance.</t>
+    <t>What are the required files in uploading a Payment Screenshot?</t>
+  </si>
+  <si>
+    <t>We accept JPG, JPEG, PNG, and HEIC file formats for image uploads.</t>
+  </si>
+  <si>
+    <t>What time is your check in and check out?</t>
+  </si>
+  <si>
+    <t>Check-in time is at 4:00 PM and Check-out is at 12:00 NN.</t>
+  </si>
+  <si>
+    <t>Are pets allowed during our stay in your resort?</t>
+  </si>
+  <si>
+    <t>Yes, pets are allowed but owners must be responsible for cleaning up after them.</t>
+  </si>
+  <si>
+    <t>Are there any restrictions on bringing outside food and drinks?</t>
+  </si>
+  <si>
+    <t>There are no restrictions on bringing outside food and drinks.</t>
+  </si>
+  <si>
+    <t>Does resort offer wifi? Is it free or there are additional fee?</t>
+  </si>
+  <si>
+    <t>Yes, we offer free WiFi for guests who have completed their booking, though coverage may be limited in some areas.</t>
+  </si>
+  <si>
+    <t>What are the payment methods? Do you accept full cash?</t>
+  </si>
+  <si>
+    <t>We require 50% initial payment through online wallets like GCash. The remaining balance can be settled in cash upon arrival.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -55,17 +73,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -82,8 +111,15 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -300,7 +336,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="35.5"/>
+    <col customWidth="1" min="1" max="1" width="51.63"/>
     <col customWidth="1" min="2" max="2" width="39.0"/>
   </cols>
   <sheetData>
@@ -316,25 +352,97 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>